<commit_message>
Update data package at: 2023-09-25T09:44:04Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_classificacao_receita.xlsx
+++ b/data-raw/desc_classificacao_receita.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26920"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{62941FB7-8B7D-41A0-BE4B-AF4E146BD1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E352D21C-1C77-4692-9E6B-E9A5E3E8E5D6}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{62941FB7-8B7D-41A0-BE4B-AF4E146BD1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86273B88-889D-4C0E-B162-CD920F63DDD5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5129,7 +5129,7 @@
     <t>Outras Transferências de Recursos do Sistema Único de Saúde - SUS</t>
   </si>
   <si>
-    <t>Transferências de Recursos do Fundo Nacional do Desenvolvimento da Educação - FNDE  </t>
+    <t>Transferências de Recursos do Fundo Nacional do Desenvolvimento da Educação - FNDE</t>
   </si>
   <si>
     <t>Transferências do Salário-Educação</t>
@@ -10319,8 +10319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3753"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A1735" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1744" sqref="B1744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51620,6 +51620,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
@@ -51636,15 +51645,6 @@
     <MediaLengthInSeconds xmlns="6f4338ef-addb-4c87-aefe-1895241b335f" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51897,11 +51897,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EEA503F-AFC3-4E20-893F-84CA094E21B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558EE736-02CD-495E-B2F4-B6C488CB6A62}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558EE736-02CD-495E-B2F4-B6C488CB6A62}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EEA503F-AFC3-4E20-893F-84CA094E21B5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>